<commit_message>
upodated BOM. changed mic, headphone jack, and other passive components
</commit_message>
<xml_diff>
--- a/soundCatcher_v1_BOM.xlsx
+++ b/soundCatcher_v1_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="100" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="38400" yWindow="-440" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="169">
   <si>
     <t>Notes</t>
   </si>
@@ -124,17 +124,420 @@
     <t>Compulsory columns highlighted in yellow</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>47uF 1206 Cap</t>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>0.1uF C0402 Cer Cap</t>
+  </si>
+  <si>
+    <t>C5, C6, C8, C9, C11, C12, C13, C14, C15, C19</t>
+  </si>
+  <si>
+    <t>C16, C18</t>
+  </si>
+  <si>
+    <t>27 pF C0402 Cer Cap</t>
+  </si>
+  <si>
+    <t>JP1, JP7, JP8</t>
+  </si>
+  <si>
+    <t>JP6</t>
+  </si>
+  <si>
+    <t>2-pin 0.1" male header (breakable)</t>
+  </si>
+  <si>
+    <t>3-pin 0.1" male header (breakable)</t>
+  </si>
+  <si>
+    <t>JP2, JP3, JP5</t>
+  </si>
+  <si>
+    <t>4-in 0.1" male header (breakable)</t>
+  </si>
+  <si>
+    <t>JP4</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SM49 4.096 MHz XTAL</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>5.6 kohm 0402 Res</t>
+  </si>
+  <si>
+    <t>R3, R4, R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>4.7 kohm 0201 Res</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8, R11, R15</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>270 ohm 0201 Res</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>430 ohm 0402 Res</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>80.6 kohm R0402 Res</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>MMBT3904LT1-NPN-SOT23-BEC</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>ISD15100 Audio IC;  LQFP48 Pkg</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C1, C10, C17</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>PRT-12639</t>
+  </si>
+  <si>
+    <t>Supplier Link</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/12639</t>
+  </si>
+  <si>
+    <t>3.5 mm TRRS Audio Jack SMT</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM31CR60J476ME19L/490-3907-1-ND/965949</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>490-3907-1-ND</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM31CR60J476ME19L</t>
+  </si>
+  <si>
+    <t>CAP CER 47UF 6.3V 20% X5R 1206</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CL05B103KP5NNNC/1276-1502-1-ND/3889588</t>
+  </si>
+  <si>
+    <t>CL05B103KP5NNNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 10000PF 10V 10% X7R 0402
+</t>
+  </si>
+  <si>
+    <t>1276-1502-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CL05C221JO5NNNC/1276-1668-1-ND/3889754</t>
+  </si>
+  <si>
+    <t>CL05C221JO5NNNC</t>
+  </si>
+  <si>
+    <t>1276-1668-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 220PF 16V 5% NP0 0402</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CC0402KRX7R7BB102/311-1352-1-ND/2103136</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R7BB102</t>
+  </si>
+  <si>
+    <t>311-1352-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 16V 10% X7R 0402</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/LMK105BJ104KV-F/587-1227-1-ND/931004</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>LMK105BJ104KV-F</t>
+  </si>
+  <si>
+    <t>587-1227-1-ND</t>
+  </si>
+  <si>
+    <t>Nichicon</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/UWX1A221MCL1GB/493-2098-1-ND/590073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP ALUM 220UF 10V 20% SMD
+</t>
+  </si>
+  <si>
+    <t>UWX1A221MCL1GB</t>
+  </si>
+  <si>
+    <t>493-2098-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM1555C1E270JA01D/490-6176-1-ND/3845376</t>
+  </si>
+  <si>
+    <t>GRM1555C1E270JA01D</t>
+  </si>
+  <si>
+    <t>490-6176-1-ND</t>
+  </si>
+  <si>
+    <t>PRT-00116</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/116</t>
+  </si>
+  <si>
+    <t>Break into either 2-pin, 3-pin, or 4-pin size</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/9C-4.096MBBK-T/887-1828-1-ND/3585944</t>
+  </si>
+  <si>
+    <t>TXC Corporation</t>
+  </si>
+  <si>
+    <t>9C-4.096MBBK-T</t>
+  </si>
+  <si>
+    <t>887-1828-1-ND</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>WM-61A</t>
+  </si>
+  <si>
+    <t>Electret Microphone SMD; 20~20kHz</t>
+  </si>
+  <si>
+    <t>ebay</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/like/350779217336?lpid=82</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CKN9104CT-ND</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>C&amp;K Components</t>
+  </si>
+  <si>
+    <t>PTS525SM10SMTR LFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset Button; SWITCH TACTILE SPST-NO 0.05A 12V
+</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/PTS525SM10SMTR%20LFS/CKN9104CT-ND/1146923</t>
+  </si>
+  <si>
+    <t>MMBT3904FSCT-ND</t>
+  </si>
+  <si>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>TRANSISTOR GP NPN AMP SOT-23</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MMBT3904/MMBT3904FSCT-ND/458971</t>
+  </si>
+  <si>
+    <t>Nuvoton</t>
+  </si>
+  <si>
+    <t>ISD15102FYI-ND</t>
+  </si>
+  <si>
+    <t>ISD15102FYI</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=150829081&amp;uq=635380423261759830</t>
+  </si>
+  <si>
+    <t>Stackpole</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RMCF0402JT5K60/RMCF0402JT5K60CT-ND/2417891</t>
+  </si>
+  <si>
+    <t>RMCF0402JT5K60</t>
+  </si>
+  <si>
+    <t>RMCF0402JT5K60CT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0201JR-071K5L/311-1.5KNCT-ND/1949025</t>
+  </si>
+  <si>
+    <t>RC0201JR-071K5L</t>
+  </si>
+  <si>
+    <t>311-1.5KNCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 1.5K OHM 1/20W 5% 0201 SMD
+</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ERJ-1GNJ472C/P4.7AECT-ND/4250859</t>
+  </si>
+  <si>
+    <t>ERJ-1GNJ472C</t>
+  </si>
+  <si>
+    <t>P4.7AECT-ND</t>
+  </si>
+  <si>
+    <t>Rohm semiconductor</t>
+  </si>
+  <si>
+    <t>MCR006YRTJ101</t>
+  </si>
+  <si>
+    <t>RHM100CCCT-ND</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 1/20W 5% 0201 SMD</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MCR006YRTJ101/RHM100CCCT-ND/2796406</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1/20W 5% 0201 SMD</t>
+  </si>
+  <si>
+    <t>RC0201JR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10KNCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0201JR-0710KL/311-10KNCT-ND/1949007</t>
+  </si>
+  <si>
+    <t>ERJ-1GEJ271C</t>
+  </si>
+  <si>
+    <t>P270AGCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ERJ-1GEJ271C/P270AGCT-ND/285187</t>
+  </si>
+  <si>
+    <t>RC0201JR-071ML</t>
+  </si>
+  <si>
+    <t>311-1MNCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0201JR-071ML/311-1MNCT-ND/1949029</t>
+  </si>
+  <si>
+    <t>RES 1M OHM 1/20W 5% 0201 SMD</t>
+  </si>
+  <si>
+    <t>RC0402FR-07430RL</t>
+  </si>
+  <si>
+    <t>311-430LRCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0402FR-07430RL/311-430LRCT-ND/729558</t>
+  </si>
+  <si>
+    <t>RMCF0402FT80K6</t>
+  </si>
+  <si>
+    <t>RMCF0402FT80K6CT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RMCF0402FT80K6/RMCF0402FT80K6CT-ND/2417791</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -146,18 +549,45 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +618,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -293,11 +728,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -329,19 +825,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -350,22 +840,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -380,8 +861,90 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="7" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,116 +1245,746 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="17" customWidth="1"/>
-    <col min="3" max="3" width="36.5" style="16" customWidth="1"/>
-    <col min="4" max="5" width="24" style="16" customWidth="1"/>
-    <col min="6" max="6" width="16" style="16" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="20" style="16" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="17"/>
+    <col min="1" max="1" width="9.1640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="15" customWidth="1"/>
+    <col min="3" max="3" width="36.5" style="14" customWidth="1"/>
+    <col min="4" max="4" width="24" style="14" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="16" style="14" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="66.6640625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="20" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1">
+      <c r="A1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="35" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="15" customFormat="1">
-      <c r="A2" s="19">
+    <row r="2" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A2" s="46">
+        <v>2</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A3" s="46">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C3" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A4" s="46">
+        <v>1</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:8" s="15" customFormat="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" s="15" customFormat="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" s="15" customFormat="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" s="15" customFormat="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="23" t="s">
+      <c r="C4" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" s="13" customFormat="1" ht="36">
+      <c r="A6" s="46">
+        <v>10</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A7" s="46">
+        <v>1</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A8" s="46"/>
+      <c r="B8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A9" s="47">
+        <v>1</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="13" customFormat="1">
+      <c r="A10" s="48"/>
+      <c r="B10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" ht="13" thickBot="1">
+      <c r="A11" s="49"/>
+      <c r="B11" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="1:9" s="13" customFormat="1" ht="16" thickTop="1" thickBot="1">
+      <c r="A12" s="46">
+        <v>1</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" s="13" customFormat="1" ht="13" thickTop="1">
+      <c r="A13" s="46">
+        <v>1</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" s="13" customFormat="1">
+      <c r="A14" s="46">
+        <v>1</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A15" s="46">
+        <v>2</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A16" s="46">
+        <v>3</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:9" s="13" customFormat="1">
+      <c r="A17" s="46">
+        <v>1</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A18" s="46">
+        <v>1</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" s="13" customFormat="1">
+      <c r="A19" s="46">
+        <v>3</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="I19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" s="13" customFormat="1">
+      <c r="A20" s="46">
+        <v>1</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" s="13" customFormat="1">
+      <c r="A21" s="46">
+        <v>1</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A22" s="46">
+        <v>1</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A23" s="46">
+        <v>1</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" s="13" customFormat="1" ht="36">
+      <c r="A24" s="46">
+        <v>1</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" s="13" customFormat="1">
+      <c r="A25" s="46">
+        <v>1</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:9" s="13" customFormat="1" ht="24">
+      <c r="A26" s="46">
+        <v>1</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:9" s="13" customFormat="1">
+      <c r="A27" s="16"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="1:9" s="13" customFormat="1">
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" s="13" customFormat="1">
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+  </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.51181102362204722" right="0.4" top="0.78740157480314965" bottom="0.62992125984251968" header="0.35433070866141736" footer="0.31496062992125984"/>

</xml_diff>